<commit_message>
refactor: Remove DetailLokasiImport class and update PartsImport logging; modify routes for improved functionality
</commit_message>
<xml_diff>
--- a/public/file/format-import-part(system-sto).xlsx
+++ b/public/file/format-import-part(system-sto).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\system-sto-kbi\public\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABDA6B5B-E35E-46A2-AD39-97AFFA62B1F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5858A8A-9F13-4E8E-86BE-745C154AD051}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{235D7ECB-1AB5-47C9-9C87-335BE7A2122F}"/>
   </bookViews>
@@ -482,8 +482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4B65D39-E4F5-41EC-A577-54771F0AEB14}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>